<commit_message>
build angular in DatingApp.API
</commit_message>
<xml_diff>
--- a/FindMeApp-GANTT-WER1.xlsx
+++ b/FindMeApp-GANTT-WER1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Łukasz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Łukasz\udemy\portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37AC940E-C281-4DE2-819D-EABB057FC570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E60555-BD85-4250-9727-CCCA667160F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4360120A-B783-424C-A91F-59E9D4F124B0}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Data rozpoczęcia</t>
   </si>
@@ -57,9 +59,6 @@
     <t>3. Projekt Systemu</t>
   </si>
   <si>
-    <t>4. Implementacja</t>
-  </si>
-  <si>
     <t>5. Testowanie</t>
   </si>
   <si>
@@ -75,10 +74,10 @@
     <t>2.1 Stworzenie Wstępnego Planu Projektu</t>
   </si>
   <si>
-    <t>4.1 Implementacja wersji moblinej</t>
+    <t>4. Implementacja aplikacji .Net Core</t>
   </si>
   <si>
-    <t>4.2 Implementacja wersji WWW</t>
+    <t>4.2 Implementacja Aplikacji Angular</t>
   </si>
 </sst>
 </file>
@@ -162,10 +161,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -306,9 +305,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1. Planowanie Systemu</c:v>
                 </c:pt>
@@ -328,18 +327,15 @@
                   <c:v>3.1 Stworzenie Specyfikacji Wymagań Systemu</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4. Implementacja</c:v>
+                  <c:v>4. Implementacja aplikacji .Net Core</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1 Implementacja wersji moblinej</c:v>
+                  <c:v>4.2 Implementacja Aplikacji Angular</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2 Implementacja wersji WWW</c:v>
+                  <c:v>5. Testowanie</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5. Testowanie</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>6. Wdrożenie </c:v>
                 </c:pt>
               </c:strCache>
@@ -347,27 +343,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$13</c:f>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43758</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43758</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>43763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43763</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>43765</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>43765</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43783</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>43783</c:v>
+                  <c:v>43766</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43800</c:v>
@@ -376,12 +372,9 @@
                   <c:v>43800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43800</c:v>
+                  <c:v>43842</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43842</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>43849</c:v>
                 </c:pt>
               </c:numCache>
@@ -566,43 +559,14 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:alpha val="91000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-8291-4876-AB3D-BF73862575AE}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1. Planowanie Systemu</c:v>
                 </c:pt>
@@ -622,18 +586,15 @@
                   <c:v>3.1 Stworzenie Specyfikacji Wymagań Systemu</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4. Implementacja</c:v>
+                  <c:v>4. Implementacja aplikacji .Net Core</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1 Implementacja wersji moblinej</c:v>
+                  <c:v>4.2 Implementacja Aplikacji Angular</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2 Implementacja wersji WWW</c:v>
+                  <c:v>5. Testowanie</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5. Testowanie</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>6. Wdrożenie </c:v>
                 </c:pt>
               </c:strCache>
@@ -641,41 +602,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$13</c:f>
+              <c:f>Sheet1!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1415,13 +1373,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>533397</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>100010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>312964</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1747,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94E2B80-1D9D-46A3-8E96-85C28382198F}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,12 +1719,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1776,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -1787,14 +1745,14 @@
         <v>4</v>
       </c>
       <c r="C3" s="4">
-        <v>43758</v>
+        <v>43736</v>
       </c>
       <c r="D3" s="4">
-        <v>43764</v>
-      </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E13" si="0">D3-C3</f>
-        <v>6</v>
+        <v>43845</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E12" si="0">D3-C3</f>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1802,14 +1760,14 @@
         <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>43758</v>
+        <v>43736</v>
       </c>
       <c r="D4" s="4">
-        <v>43764</v>
-      </c>
-      <c r="E4" s="6">
+        <v>43751</v>
+      </c>
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1817,29 +1775,29 @@
         <v>6</v>
       </c>
       <c r="C5" s="4">
-        <v>43765</v>
+        <v>43763</v>
       </c>
       <c r="D5" s="4">
-        <v>43793</v>
-      </c>
-      <c r="E5" s="6">
+        <v>43780</v>
+      </c>
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
-        <v>43765</v>
+        <v>43763</v>
       </c>
       <c r="D6" s="4">
-        <v>43793</v>
-      </c>
-      <c r="E6" s="6">
+        <v>43780</v>
+      </c>
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1847,44 +1805,44 @@
         <v>7</v>
       </c>
       <c r="C7" s="4">
-        <v>43783</v>
+        <v>43765</v>
       </c>
       <c r="D7" s="4">
-        <v>43800</v>
-      </c>
-      <c r="E7" s="6">
+        <v>43777</v>
+      </c>
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43766</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43778</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
         <v>12</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43783</v>
-      </c>
-      <c r="D8" s="4">
-        <v>43800</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="0"/>
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4">
         <v>43800</v>
       </c>
       <c r="D9" s="4">
-        <v>43842</v>
-      </c>
-      <c r="E9" s="6">
+        <v>43849</v>
+      </c>
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -1895,26 +1853,26 @@
         <v>43800</v>
       </c>
       <c r="D10" s="4">
-        <v>43842</v>
-      </c>
-      <c r="E10" s="6">
+        <v>43849</v>
+      </c>
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4">
-        <v>43800</v>
+        <v>43842</v>
       </c>
       <c r="D11" s="4">
-        <v>43842</v>
-      </c>
-      <c r="E11" s="6">
+        <v>43849</v>
+      </c>
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1922,38 +1880,23 @@
         <v>9</v>
       </c>
       <c r="C12" s="4">
-        <v>43842</v>
+        <v>43849</v>
       </c>
       <c r="D12" s="4">
-        <v>43849</v>
-      </c>
-      <c r="E12" s="6">
+        <v>43856</v>
+      </c>
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4">
-        <v>43849</v>
-      </c>
-      <c r="D13" s="4">
-        <v>43856</v>
-      </c>
-      <c r="E13" s="6">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>